<commit_message>
Added titles for new Festival alts of Gold City and Symboli Rudolf
</commit_message>
<xml_diff>
--- a/xls/UmaMusume Uma Title Translation List.xlsx
+++ b/xls/UmaMusume Uma Title Translation List.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\starg\Documents\GitHub\umacruise-english-patch\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F359BA-8C89-44BF-A047-7CD3B238374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A62852C-D5AD-4AF4-A7B1-2BFAD70AD69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25500" yWindow="360" windowWidth="15300" windowHeight="7875" xr2:uid="{256B361F-8AF2-4BD7-A250-3B4078BE616F}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{256B361F-8AF2-4BD7-A250-3B4078BE616F}"/>
   </bookViews>
   <sheets>
     <sheet name="uma-title" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'uma-title'!$A$1:$B$52</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'uma-title'!$A$1:$B$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>text</t>
   </si>
@@ -332,6 +332,18 @@
   </si>
   <si>
     <t>シューティンスタァ・ルヴュ</t>
+  </si>
+  <si>
+    <t>秋桜ダンツァトリーチェ</t>
+  </si>
+  <si>
+    <t>Akizakura Danzatrice</t>
+  </si>
+  <si>
+    <t>Archer of the White Moon</t>
+  </si>
+  <si>
+    <t>皓月の弓取り</t>
   </si>
 </sst>
 </file>
@@ -406,7 +418,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F87C1720-EBC1-4D75-8EF8-73897E92E54D}" name="uma_title" displayName="uma_title" ref="A1:B52" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F87C1720-EBC1-4D75-8EF8-73897E92E54D}" name="uma_title" displayName="uma_title" ref="A1:B54" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F332A4BD-E5A7-454A-A0F4-614F4188483E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{66B0ABE4-20FB-4E98-AA9D-0F05E3D3244F}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
@@ -712,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6952997-12D1-4644-9DFE-1443916FDD50}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,6 +1150,22 @@
       </c>
       <c r="B52" s="1" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>